<commit_message>
Completed subject reconciliation and prepared for production ingest
</commit_message>
<xml_diff>
--- a/mss0080/CLR/CLR_standard_input_mss0080.xlsx
+++ b/mss0080/CLR/CLR_standard_input_mss0080.xlsx
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="647">
   <si>
     <t>text</t>
   </si>
@@ -2093,16 +2093,19 @@
     <t>William Bond Papers @ http://library.ucsd.edu/speccoll/findingaids/mss0080.html</t>
   </si>
   <si>
-    <t>Bond, William, d. 1776 -- Archives | Washington, George, 1732-1799</t>
-  </si>
-  <si>
     <t>Massachusetts. Provincial Congress</t>
   </si>
   <si>
-    <t>Regimental histories -- Massachusetts | United States. Continental Army. Massachussetts Regiment, 25th | United States -- History -- Revolution, 1775-1783</t>
-  </si>
-  <si>
     <t>m80b1f26i1p1.tif</t>
+  </si>
+  <si>
+    <t>Bond, William, d. 1776  | Washington, George, 1732-1799</t>
+  </si>
+  <si>
+    <t>Massachusetts</t>
+  </si>
+  <si>
+    <t>Regimental histories | United States. Continental Army. | United States. Continental Army. Massachussetts Regiment, 25th | History | American Revolution (1775-1783)</t>
   </si>
 </sst>
 </file>
@@ -3151,10 +3154,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3170,11 +3173,11 @@
     <col min="9" max="9" width="15.140625" style="3" customWidth="1"/>
     <col min="10" max="10" width="19.85546875" style="3" customWidth="1"/>
     <col min="11" max="12" width="39.140625" style="3" customWidth="1"/>
-    <col min="13" max="16" width="42.85546875" style="3" customWidth="1"/>
-    <col min="17" max="17" width="84.28515625" style="3" customWidth="1"/>
+    <col min="13" max="17" width="42.85546875" style="3" customWidth="1"/>
+    <col min="18" max="18" width="84.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>337</v>
       </c>
@@ -3221,18 +3224,21 @@
         <v>459</v>
       </c>
       <c r="P1" s="16" t="s">
+        <v>454</v>
+      </c>
+      <c r="Q1" s="16" t="s">
         <v>450</v>
       </c>
-      <c r="Q1" s="16" t="s">
+      <c r="R1" s="16" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="24" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" s="24" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>631</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C2" s="23" t="s">
         <v>0</v>
@@ -3265,18 +3271,21 @@
         <v>639</v>
       </c>
       <c r="M2" s="23" t="s">
+        <v>644</v>
+      </c>
+      <c r="N2" s="23" t="s">
         <v>642</v>
       </c>
-      <c r="N2" s="23" t="s">
-        <v>643</v>
-      </c>
       <c r="O2" s="23" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="P2" s="23" t="s">
+        <v>645</v>
+      </c>
+      <c r="Q2" s="23" t="s">
         <v>640</v>
       </c>
-      <c r="Q2" s="23" t="s">
+      <c r="R2" s="23" t="s">
         <v>641</v>
       </c>
     </row>
@@ -3318,13 +3327,13 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$G$1:$G$17</xm:f>
           </x14:formula1>
-          <xm:sqref>M1:O1 P1</xm:sqref>
+          <xm:sqref>M1:P1 Q1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$I$1:$I$12</xm:f>
           </x14:formula1>
-          <xm:sqref>Q1</xm:sqref>
+          <xm:sqref>R1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>

</xml_diff>